<commit_message>
datos arreglados, grafos y caso basa. También coordenadas de costos y madera
</commit_message>
<xml_diff>
--- a/data/costos_y_madera_nodos.xlsx
+++ b/data/costos_y_madera_nodos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/mswahl_uc_cl/Documents/Documentos/Universidad/2025/2025-1/Capston/capstone_industrial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{A6325F13-CECA-4D4F-89BA-8CC1BAF2FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED8351B3-73D8-4102-99A5-4AA7D921BDCE}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{A6325F13-CECA-4D4F-89BA-8CC1BAF2FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{812FF7BD-EB6A-4A6D-B765-D628E50C81D2}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{FB2FC1B4-D5CD-4D1E-8ADB-DFA80849F99B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FB2FC1B4-D5CD-4D1E-8ADB-DFA80849F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="5" r:id="rId1"/>
@@ -442,8 +442,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602BFF83-F3F6-4A8A-B350-5D6608CEEF1F}">
   <dimension ref="A1:G211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D212" sqref="D212"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G168" sqref="G168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3775,7 +3776,7 @@
         <v>14</v>
       </c>
       <c r="D153">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E153" t="s">
         <v>8</v>
@@ -3798,7 +3799,7 @@
         <v>15</v>
       </c>
       <c r="D154">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F154">
         <v>0</v>
@@ -3841,7 +3842,7 @@
         <v>13</v>
       </c>
       <c r="D156">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E156" t="s">
         <v>8</v>
@@ -3864,7 +3865,7 @@
         <v>14</v>
       </c>
       <c r="D157">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E157" t="s">
         <v>8</v>
@@ -3887,7 +3888,7 @@
         <v>15</v>
       </c>
       <c r="D158">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E158" t="s">
         <v>8</v>
@@ -3956,7 +3957,7 @@
         <v>13</v>
       </c>
       <c r="D161">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E161" t="s">
         <v>8</v>
@@ -3979,7 +3980,7 @@
         <v>14</v>
       </c>
       <c r="D162">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E162" t="s">
         <v>8</v>
@@ -4002,7 +4003,7 @@
         <v>15</v>
       </c>
       <c r="D163">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E163" t="s">
         <v>8</v>
@@ -4071,7 +4072,7 @@
         <v>14</v>
       </c>
       <c r="D166">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E166" t="s">
         <v>8</v>
@@ -4094,7 +4095,7 @@
         <v>15</v>
       </c>
       <c r="D167">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E167" t="s">
         <v>8</v>
@@ -4163,7 +4164,7 @@
         <v>15</v>
       </c>
       <c r="D170">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E170" t="s">
         <v>8</v>
@@ -4186,7 +4187,7 @@
         <v>11</v>
       </c>
       <c r="D171">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E171" t="s">
         <v>8</v>
@@ -4209,7 +4210,7 @@
         <v>11</v>
       </c>
       <c r="D172">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E172" t="s">
         <v>8</v>
@@ -4232,7 +4233,7 @@
         <v>12</v>
       </c>
       <c r="D173">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E173" t="s">
         <v>8</v>
@@ -4301,7 +4302,7 @@
         <v>13</v>
       </c>
       <c r="D176">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E176" t="s">
         <v>8</v>
@@ -4324,7 +4325,7 @@
         <v>14</v>
       </c>
       <c r="D177">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E177" t="s">
         <v>8</v>
@@ -4347,7 +4348,7 @@
         <v>15</v>
       </c>
       <c r="D178">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E178" t="s">
         <v>8</v>
@@ -4416,7 +4417,7 @@
         <v>13</v>
       </c>
       <c r="D181">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E181" t="s">
         <v>8</v>
@@ -4439,7 +4440,7 @@
         <v>14</v>
       </c>
       <c r="D182">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E182" t="s">
         <v>8</v>
@@ -4462,7 +4463,7 @@
         <v>15</v>
       </c>
       <c r="D183">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E183" t="s">
         <v>8</v>
@@ -4531,7 +4532,7 @@
         <v>13</v>
       </c>
       <c r="D186">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E186" t="s">
         <v>8</v>
@@ -4554,7 +4555,7 @@
         <v>14</v>
       </c>
       <c r="D187">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E187" t="s">
         <v>8</v>
@@ -4577,7 +4578,7 @@
         <v>15</v>
       </c>
       <c r="D188">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E188" t="s">
         <v>8</v>
@@ -4623,7 +4624,7 @@
         <v>13</v>
       </c>
       <c r="D190">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E190" t="s">
         <v>8</v>
@@ -4646,7 +4647,7 @@
         <v>14</v>
       </c>
       <c r="D191">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E191" t="s">
         <v>8</v>
@@ -4669,7 +4670,7 @@
         <v>15</v>
       </c>
       <c r="D192">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E192" t="s">
         <v>8</v>
@@ -4715,7 +4716,7 @@
         <v>13</v>
       </c>
       <c r="D194">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E194" t="s">
         <v>8</v>
@@ -4738,7 +4739,7 @@
         <v>14</v>
       </c>
       <c r="D195">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E195" t="s">
         <v>8</v>
@@ -4761,7 +4762,7 @@
         <v>15</v>
       </c>
       <c r="D196">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E196" t="s">
         <v>8</v>
@@ -4807,7 +4808,7 @@
         <v>13</v>
       </c>
       <c r="D198">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E198" t="s">
         <v>8</v>
@@ -4830,7 +4831,7 @@
         <v>14</v>
       </c>
       <c r="D199">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E199" t="s">
         <v>8</v>
@@ -4853,7 +4854,7 @@
         <v>15</v>
       </c>
       <c r="D200">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E200" t="s">
         <v>8</v>
@@ -4899,7 +4900,7 @@
         <v>12</v>
       </c>
       <c r="D202">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E202" t="s">
         <v>8</v>
@@ -4922,7 +4923,7 @@
         <v>13</v>
       </c>
       <c r="D203">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E203" t="s">
         <v>8</v>
@@ -4945,7 +4946,7 @@
         <v>14</v>
       </c>
       <c r="D204">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E204" t="s">
         <v>8</v>
@@ -4991,7 +4992,7 @@
         <v>12</v>
       </c>
       <c r="D206">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E206" t="s">
         <v>8</v>
@@ -5014,7 +5015,7 @@
         <v>13</v>
       </c>
       <c r="D207">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E207" t="s">
         <v>8</v>
@@ -5037,7 +5038,7 @@
         <v>14</v>
       </c>
       <c r="D208">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E208" t="s">
         <v>8</v>
@@ -5083,7 +5084,7 @@
         <v>12</v>
       </c>
       <c r="D210">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E210" t="s">
         <v>8</v>
@@ -5106,7 +5107,7 @@
         <v>13</v>
       </c>
       <c r="D211">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E211" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Funciona pero no sirve
</commit_message>
<xml_diff>
--- a/data/costos_y_madera_nodos.xlsx
+++ b/data/costos_y_madera_nodos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/tgoas_uc_cl/Documents/Documentos/PUC/9no sem/Capstone/capstone_industrial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{A6325F13-CECA-4D4F-89BA-8CC1BAF2FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CD8F4A8-E91C-43C0-9BA3-960D69DDFE5C}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{A6325F13-CECA-4D4F-89BA-8CC1BAF2FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C957D3C8-60A5-4C70-81DA-78B61417F173}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{FB2FC1B4-D5CD-4D1E-8ADB-DFA80849F99B}"/>
   </bookViews>
@@ -438,8 +438,8 @@
   <dimension ref="A1:K211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J142" sqref="J142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>550.29499999999996</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -553,7 +553,7 @@
         <v>15000</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>606.70000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -639,7 +639,7 @@
         <v>15000</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>583.5</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -726,7 +726,7 @@
         <v>15000</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>602.4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -815,7 +815,7 @@
         <v>15000</v>
       </c>
       <c r="G17">
-        <v>15</v>
+        <v>552.6</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>509.8</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -988,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>663.3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1054,7 +1054,7 @@
         <v>45000</v>
       </c>
       <c r="G28">
-        <v>45</v>
+        <v>586.9</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>699.8</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>514.9</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1246,7 +1246,7 @@
         <v>45000</v>
       </c>
       <c r="G37">
-        <v>45</v>
+        <v>576</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1312,7 +1312,7 @@
         <v>55000</v>
       </c>
       <c r="G40">
-        <v>55</v>
+        <v>670.6</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1378,7 +1378,7 @@
         <v>40000</v>
       </c>
       <c r="G43">
-        <v>40</v>
+        <v>609.5</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>550.29499999999996</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>550.29499999999996</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>532.79999999999995</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -2358,7 +2358,7 @@
         <v>5000</v>
       </c>
       <c r="G90">
-        <v>5</v>
+        <v>473.625</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -3803,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="G154">
-        <v>0</v>
+        <v>550.29499999999996</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
excel costos con volumen de madera 0
</commit_message>
<xml_diff>
--- a/data/costos_y_madera_nodos.xlsx
+++ b/data/costos_y_madera_nodos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/tgoas_uc_cl/Documents/Documentos/PUC/9no sem/Capstone/capstone_industrial/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/mswahl_uc_cl/Documents/Documentos/Universidad/2025/2025-1/Capston/capstone_industrial/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{A6325F13-CECA-4D4F-89BA-8CC1BAF2FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C957D3C8-60A5-4C70-81DA-78B61417F173}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{A6325F13-CECA-4D4F-89BA-8CC1BAF2FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ECD4B1F-B307-44BE-8074-178C301CD2C2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{FB2FC1B4-D5CD-4D1E-8ADB-DFA80849F99B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FB2FC1B4-D5CD-4D1E-8ADB-DFA80849F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="5" r:id="rId1"/>
@@ -435,11 +435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602BFF83-F3F6-4A8A-B350-5D6608CEEF1F}">
-  <dimension ref="A1:K211"/>
+  <dimension ref="A1:K216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J142" sqref="J142"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I216" sqref="I216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>550.29499999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>550.29499999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>550.29499999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -3803,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="G154">
-        <v>550.29499999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
@@ -5048,7 +5048,7 @@
         <v>431.9</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>208</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>589.4</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>209</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>631.1</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>210</v>
       </c>
@@ -5116,6 +5116,9 @@
       <c r="G211">
         <v>605.5</v>
       </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I216" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G211" xr:uid="{602BFF83-F3F6-4A8A-B350-5D6608CEEF1F}"/>

</xml_diff>